<commit_message>
CrewAI Robust Backend Ready!
</commit_message>
<xml_diff>
--- a/Data_processed/electricity/electricity Canada.xlsx
+++ b/Data_processed/electricity/electricity Canada.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -122,6 +134,51 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/comments/comment1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Data Processor</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <t>Data type: Categorical (text)</t>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <t>Data type: Various (e.g. kg, kWh)</t>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <t>Data type: Categorical (text)</t>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <t>Data type: Carbon footprint</t>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <t>Data type: Cumulative energy demand</t>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <t>Data type: Climate change impact</t>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0">
+      <text>
+        <t>Data type: Categorical (text)</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -413,14 +470,456 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>industry</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>process</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>carbon (kg CO2 eq)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>ced (MJ)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>climate change (kg CO2 eq)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>region</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>electricity Canada</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MJ </t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Electricity Alberta production</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.1832334</v>
+      </c>
+      <c r="E2" t="n">
+        <v>5.1696617</v>
+      </c>
+      <c r="F2" t="n">
+        <v>5.1090334e-06</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>electricity Canada</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MJ </t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Electricity British Columbia production</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.007710413333333334</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2.7146856</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2.1498678e-07</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>electricity Canada</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MJ </t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Electricity Manitoba production</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.002696516133333333</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2.4069924</v>
+      </c>
+      <c r="F4" t="n">
+        <v>7.518602499999999e-08</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>electricity Canada</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MJ </t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Electricity New Brunswick production</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.1172720733333334</v>
+      </c>
+      <c r="E5" t="n">
+        <v>5.4198524</v>
+      </c>
+      <c r="F5" t="n">
+        <v>3.2698565e-06</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>electricity Canada</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MJ </t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Electricity Newfoundland and Labrador production</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.008116472000000001</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2.4751724</v>
+      </c>
+      <c r="F6" t="n">
+        <v>2.2630878e-07</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>electricity Canada</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MJ </t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Electricity Northwest Territories production</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.07082859333333334</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3.3732382</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1.974889e-06</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>electricity Canada</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MJ </t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Electricity Nova Scotia production</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.23382572</v>
+      </c>
+      <c r="E8" t="n">
+        <v>5.5935083</v>
+      </c>
+      <c r="F8" t="n">
+        <v>6.5196815e-06</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>electricity Canada</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MJ </t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Electricity Nunavut production</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.2623447066666667</v>
+      </c>
+      <c r="E9" t="n">
+        <v>6.807562</v>
+      </c>
+      <c r="F9" t="n">
+        <v>7.3148665e-06</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>electricity Canada</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MJ </t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Electricity Ontario production</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.01747998866666667</v>
+      </c>
+      <c r="E10" t="n">
+        <v>5.2048931</v>
+      </c>
+      <c r="F10" t="n">
+        <v>4.8738847e-07</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>electricity Canada</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MJ </t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Electricity Prince Edward Island production</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.1090852666666667</v>
+      </c>
+      <c r="E11" t="n">
+        <v>2.4378196</v>
+      </c>
+      <c r="F11" t="n">
+        <v>3.0415866e-06</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>electricity Canada</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MJ </t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Electricity Quebec production</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.002762364733333334</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2.4289887</v>
+      </c>
+      <c r="F12" t="n">
+        <v>7.7022058e-08</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>electricity Canada</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MJ </t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Electricity Saskatchewan production</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.23363732</v>
+      </c>
+      <c r="E13" t="n">
+        <v>5.4935004</v>
+      </c>
+      <c r="F13" t="n">
+        <v>6.5144284e-06</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>electricity Canada</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MJ </t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Electricity Yukon production</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0.03169615533333334</v>
+      </c>
+      <c r="E14" t="n">
+        <v>3.3269108</v>
+      </c>
+      <c r="F14" t="n">
+        <v>8.8377292e-07</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
</xml_diff>